<commit_message>
🔧 MAJ app.py, README.md, JSON & requirements.txt, nettoyage data obsolète
</commit_message>
<xml_diff>
--- a/data/ingredients_nettoyes_et_standardises.xlsx
+++ b/data/ingredients_nettoyes_et_standardises.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yamine\Documents\fiche-technique-streamlit\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40BC4C8-2BFD-4973-97BE-D40BD4038CD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD127C0-E23D-470B-B56E-0DA58FE36187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="21468" windowHeight="11988" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1193" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1190" uniqueCount="126">
   <si>
     <t>plat</t>
   </si>
@@ -356,9 +356,6 @@
   </si>
   <si>
     <t>Carbonara</t>
-  </si>
-  <si>
-    <t>vin blanc</t>
   </si>
   <si>
     <t>Fermière</t>
@@ -768,10 +765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F397"/>
+  <dimension ref="A1:F396"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A379" workbookViewId="0">
-      <selection activeCell="G396" sqref="G396"/>
+    <sheetView tabSelected="1" topLeftCell="A353" workbookViewId="0">
+      <selection activeCell="H369" sqref="H369"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3101,7 +3098,7 @@
         <v>25</v>
       </c>
       <c r="B137" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C137">
         <v>5</v>
@@ -3169,7 +3166,7 @@
         <v>26</v>
       </c>
       <c r="B141" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C141">
         <v>5</v>
@@ -5971,7 +5968,7 @@
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B306" t="s">
         <v>102</v>
@@ -5988,7 +5985,7 @@
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B307" t="s">
         <v>104</v>
@@ -6005,7 +6002,7 @@
     </row>
     <row r="308" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B308" t="s">
         <v>87</v>
@@ -6022,7 +6019,7 @@
     </row>
     <row r="309" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B309" t="s">
         <v>101</v>
@@ -6039,7 +6036,7 @@
     </row>
     <row r="310" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B310" t="s">
         <v>100</v>
@@ -6481,7 +6478,7 @@
     </row>
     <row r="336" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B336" t="s">
         <v>87</v>
@@ -6498,7 +6495,7 @@
     </row>
     <row r="337" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B337" t="s">
         <v>101</v>
@@ -6515,7 +6512,7 @@
     </row>
     <row r="338" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B338" t="s">
         <v>100</v>
@@ -6532,7 +6529,7 @@
     </row>
     <row r="339" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B339" t="s">
         <v>77</v>
@@ -6549,7 +6546,7 @@
     </row>
     <row r="340" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B340" t="s">
         <v>104</v>
@@ -6566,7 +6563,7 @@
     </row>
     <row r="341" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B341" t="s">
         <v>77</v>
@@ -6583,7 +6580,7 @@
     </row>
     <row r="342" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B342" t="s">
         <v>100</v>
@@ -6600,7 +6597,7 @@
     </row>
     <row r="343" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B343" t="s">
         <v>101</v>
@@ -6617,7 +6614,7 @@
     </row>
     <row r="344" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B344" t="s">
         <v>98</v>
@@ -6634,7 +6631,7 @@
     </row>
     <row r="345" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B345" t="s">
         <v>87</v>
@@ -6651,7 +6648,7 @@
     </row>
     <row r="346" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B346" t="s">
         <v>97</v>
@@ -6668,7 +6665,7 @@
     </row>
     <row r="347" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B347" t="s">
         <v>85</v>
@@ -6773,7 +6770,7 @@
         <v>107</v>
       </c>
       <c r="B353" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C353">
         <v>210</v>
@@ -6858,7 +6855,7 @@
         <v>108</v>
       </c>
       <c r="B358" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C358">
         <v>210</v>
@@ -6926,7 +6923,7 @@
         <v>67</v>
       </c>
       <c r="B362" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C362">
         <v>230</v>
@@ -6977,13 +6974,16 @@
         <v>111</v>
       </c>
       <c r="B365" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="C365">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D365" t="s">
         <v>105</v>
+      </c>
+      <c r="E365">
+        <v>15.25</v>
       </c>
     </row>
     <row r="366" spans="1:5" x14ac:dyDescent="0.3">
@@ -6991,101 +6991,101 @@
         <v>111</v>
       </c>
       <c r="B366" t="s">
-        <v>77</v>
+        <v>122</v>
       </c>
       <c r="C366">
-        <v>10</v>
+        <v>230</v>
       </c>
       <c r="D366" t="s">
         <v>105</v>
       </c>
       <c r="E366">
-        <v>15.25</v>
+        <v>2.4500000000000002</v>
       </c>
     </row>
     <row r="367" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A367" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B367" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="C367">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="D367" t="s">
         <v>105</v>
       </c>
       <c r="E367">
-        <v>2.4500000000000002</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="368" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A368" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B368" t="s">
-        <v>109</v>
+        <v>74</v>
       </c>
       <c r="C368">
-        <v>220</v>
+        <v>78</v>
       </c>
       <c r="D368" t="s">
         <v>105</v>
       </c>
       <c r="E368">
-        <v>3.3</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="369" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A369" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B369" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C369">
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="D369" t="s">
         <v>105</v>
       </c>
       <c r="E369">
-        <v>5.5</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="370" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A370" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B370" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C370">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="D370" t="s">
         <v>105</v>
       </c>
       <c r="E370">
-        <v>3.3</v>
+        <v>15.25</v>
       </c>
     </row>
     <row r="371" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A371" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B371" t="s">
-        <v>77</v>
+        <v>122</v>
       </c>
       <c r="C371">
-        <v>10</v>
+        <v>210</v>
       </c>
       <c r="D371" t="s">
         <v>105</v>
       </c>
       <c r="E371">
-        <v>15.25</v>
+        <v>2.4500000000000002</v>
       </c>
     </row>
     <row r="372" spans="1:5" x14ac:dyDescent="0.3">
@@ -7093,67 +7093,67 @@
         <v>113</v>
       </c>
       <c r="B372" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="C372">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="D372" t="s">
         <v>105</v>
       </c>
       <c r="E372">
-        <v>2.4500000000000002</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="373" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A373" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B373" t="s">
-        <v>109</v>
+        <v>72</v>
       </c>
       <c r="C373">
-        <v>220</v>
+        <v>35</v>
       </c>
       <c r="D373" t="s">
         <v>105</v>
       </c>
       <c r="E373">
-        <v>3.3</v>
+        <v>8.35</v>
       </c>
     </row>
     <row r="374" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A374" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B374" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C374">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="D374" t="s">
         <v>105</v>
       </c>
       <c r="E374">
-        <v>8.35</v>
+        <v>15.25</v>
       </c>
     </row>
     <row r="375" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A375" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B375" t="s">
-        <v>77</v>
+        <v>122</v>
       </c>
       <c r="C375">
-        <v>20</v>
+        <v>230</v>
       </c>
       <c r="D375" t="s">
         <v>105</v>
       </c>
       <c r="E375">
-        <v>15.25</v>
+        <v>2.4500000000000002</v>
       </c>
     </row>
     <row r="376" spans="1:5" x14ac:dyDescent="0.3">
@@ -7161,169 +7161,169 @@
         <v>114</v>
       </c>
       <c r="B376" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="C376">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="D376" t="s">
         <v>105</v>
       </c>
       <c r="E376">
-        <v>2.4500000000000002</v>
+        <v>2.63</v>
       </c>
     </row>
     <row r="377" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A377" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B377" t="s">
         <v>116</v>
       </c>
       <c r="C377">
-        <v>205</v>
+        <v>5</v>
       </c>
       <c r="D377" t="s">
         <v>105</v>
       </c>
       <c r="E377">
-        <v>2.63</v>
+        <v>10.67</v>
       </c>
     </row>
     <row r="378" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A378" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B378" t="s">
-        <v>117</v>
+        <v>87</v>
       </c>
       <c r="C378">
+        <v>44</v>
+      </c>
+      <c r="D378" t="s">
+        <v>105</v>
+      </c>
+      <c r="E378">
         <v>5</v>
-      </c>
-      <c r="D378" t="s">
-        <v>105</v>
-      </c>
-      <c r="E378">
-        <v>10.67</v>
       </c>
     </row>
     <row r="379" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A379" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B379" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C379">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="D379" t="s">
         <v>105</v>
       </c>
       <c r="E379">
-        <v>5</v>
+        <v>15.25</v>
       </c>
     </row>
     <row r="380" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A380" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B380" t="s">
-        <v>77</v>
+        <v>122</v>
       </c>
       <c r="C380">
-        <v>10</v>
+        <v>230</v>
       </c>
       <c r="D380" t="s">
         <v>105</v>
       </c>
       <c r="E380">
-        <v>15.25</v>
+        <v>2.4500000000000002</v>
       </c>
     </row>
     <row r="381" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A381" t="s">
+        <v>117</v>
+      </c>
+      <c r="B381" t="s">
         <v>115</v>
       </c>
-      <c r="B381" t="s">
-        <v>123</v>
-      </c>
       <c r="C381">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="D381" t="s">
         <v>105</v>
       </c>
       <c r="E381">
-        <v>2.4500000000000002</v>
+        <v>2.63</v>
       </c>
     </row>
     <row r="382" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A382" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B382" t="s">
-        <v>116</v>
+        <v>87</v>
       </c>
       <c r="C382">
-        <v>205</v>
+        <v>44</v>
       </c>
       <c r="D382" t="s">
         <v>105</v>
       </c>
       <c r="E382">
-        <v>2.63</v>
+        <v>5</v>
       </c>
     </row>
     <row r="383" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A383" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B383" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C383">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="D383" t="s">
         <v>105</v>
       </c>
       <c r="E383">
-        <v>5</v>
+        <v>5.35</v>
       </c>
     </row>
     <row r="384" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A384" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B384" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="C384">
-        <v>62</v>
+        <v>10</v>
       </c>
       <c r="D384" t="s">
         <v>105</v>
       </c>
       <c r="E384">
-        <v>5.35</v>
+        <v>15.25</v>
       </c>
     </row>
     <row r="385" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A385" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B385" t="s">
-        <v>77</v>
+        <v>122</v>
       </c>
       <c r="C385">
-        <v>10</v>
+        <v>210</v>
       </c>
       <c r="D385" t="s">
         <v>105</v>
       </c>
       <c r="E385">
-        <v>15.25</v>
+        <v>2.4500000000000002</v>
       </c>
     </row>
     <row r="386" spans="1:5" x14ac:dyDescent="0.3">
@@ -7331,41 +7331,41 @@
         <v>118</v>
       </c>
       <c r="B386" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="C386">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="D386" t="s">
         <v>105</v>
       </c>
       <c r="E386">
-        <v>2.4500000000000002</v>
+        <v>2.63</v>
       </c>
     </row>
     <row r="387" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A387" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B387" t="s">
         <v>116</v>
       </c>
       <c r="C387">
-        <v>205</v>
+        <v>5</v>
       </c>
       <c r="D387" t="s">
         <v>105</v>
       </c>
       <c r="E387">
-        <v>2.63</v>
+        <v>10.67</v>
       </c>
     </row>
     <row r="388" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A388" t="s">
+        <v>118</v>
+      </c>
+      <c r="B388" t="s">
         <v>119</v>
-      </c>
-      <c r="B388" t="s">
-        <v>117</v>
       </c>
       <c r="C388">
         <v>5</v>
@@ -7374,52 +7374,52 @@
         <v>105</v>
       </c>
       <c r="E388">
-        <v>10.67</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="389" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A389" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B389" t="s">
-        <v>120</v>
+        <v>77</v>
       </c>
       <c r="C389">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D389" t="s">
         <v>105</v>
       </c>
       <c r="E389">
-        <v>2.4</v>
+        <v>15.25</v>
       </c>
     </row>
     <row r="390" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A390" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B390" t="s">
-        <v>77</v>
+        <v>122</v>
       </c>
       <c r="C390">
-        <v>10</v>
+        <v>230</v>
       </c>
       <c r="D390" t="s">
         <v>105</v>
       </c>
       <c r="E390">
-        <v>15.25</v>
+        <v>2.4500000000000002</v>
       </c>
     </row>
     <row r="391" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A391" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B391" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C391">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="D391" t="s">
         <v>105</v>
@@ -7430,103 +7430,86 @@
     </row>
     <row r="392" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A392" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B392" t="s">
-        <v>123</v>
+        <v>77</v>
       </c>
       <c r="C392">
-        <v>210</v>
+        <v>10</v>
       </c>
       <c r="D392" t="s">
         <v>105</v>
       </c>
       <c r="E392">
-        <v>2.4500000000000002</v>
+        <v>15.25</v>
       </c>
     </row>
     <row r="393" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A393" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B393" t="s">
-        <v>77</v>
+        <v>119</v>
       </c>
       <c r="C393">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D393" t="s">
         <v>105</v>
       </c>
       <c r="E393">
-        <v>15.25</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="394" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A394" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B394" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C394">
-        <v>5</v>
+        <v>205</v>
       </c>
       <c r="D394" t="s">
         <v>105</v>
       </c>
       <c r="E394">
-        <v>2.4</v>
+        <v>2.63</v>
       </c>
     </row>
     <row r="395" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A395" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B395" t="s">
-        <v>116</v>
+        <v>74</v>
       </c>
       <c r="C395">
-        <v>205</v>
+        <v>78</v>
       </c>
       <c r="D395" t="s">
         <v>105</v>
       </c>
       <c r="E395">
-        <v>2.63</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="396" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A396" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B396" t="s">
-        <v>74</v>
+        <v>116</v>
       </c>
       <c r="C396">
-        <v>78</v>
+        <v>5</v>
       </c>
       <c r="D396" t="s">
         <v>105</v>
       </c>
       <c r="E396">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="397" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A397" t="s">
-        <v>126</v>
-      </c>
-      <c r="B397" t="s">
-        <v>117</v>
-      </c>
-      <c r="C397">
-        <v>5</v>
-      </c>
-      <c r="D397" t="s">
-        <v>105</v>
-      </c>
-      <c r="E397">
         <v>10.67</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix responsive KPI cards + mise à jour CSS
</commit_message>
<xml_diff>
--- a/data/ingredients_nettoyes_et_standardises.xlsx
+++ b/data/ingredients_nettoyes_et_standardises.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yamine\Documents\fiche-technique-streamlit\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD127C0-E23D-470B-B56E-0DA58FE36187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE17105-D48E-495C-B75A-7A0D8BA03F6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1190" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1190" uniqueCount="125">
   <si>
     <t>plat</t>
   </si>
@@ -296,9 +296,6 @@
   </si>
   <si>
     <t>sauce tomate</t>
-  </si>
-  <si>
-    <t>Soubressade</t>
   </si>
   <si>
     <t xml:space="preserve">Jambon blanc (Dinde) </t>
@@ -767,8 +764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F396"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A353" workbookViewId="0">
-      <selection activeCell="H369" sqref="H369"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="H124" sqref="H124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -809,7 +806,7 @@
         <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E2">
         <v>3.75</v>
@@ -826,7 +823,7 @@
         <v>90</v>
       </c>
       <c r="D3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E3">
         <v>5.85</v>
@@ -843,7 +840,7 @@
         <v>45</v>
       </c>
       <c r="D4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E4">
         <v>15.9</v>
@@ -860,7 +857,7 @@
         <v>33</v>
       </c>
       <c r="D5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E5">
         <v>0.6</v>
@@ -877,7 +874,7 @@
         <v>70</v>
       </c>
       <c r="D6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E6">
         <v>1.2</v>
@@ -894,7 +891,7 @@
         <v>90</v>
       </c>
       <c r="D7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E7">
         <v>3.75</v>
@@ -911,7 +908,7 @@
         <v>120</v>
       </c>
       <c r="D8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E8">
         <v>5.85</v>
@@ -928,7 +925,7 @@
         <v>55</v>
       </c>
       <c r="D9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E9">
         <v>15.9</v>
@@ -945,7 +942,7 @@
         <v>45</v>
       </c>
       <c r="D10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E10">
         <v>0.6</v>
@@ -962,7 +959,7 @@
         <v>80</v>
       </c>
       <c r="D11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E11">
         <v>1.2</v>
@@ -979,7 +976,7 @@
         <v>45</v>
       </c>
       <c r="D12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E12">
         <v>3.75</v>
@@ -996,7 +993,7 @@
         <v>90</v>
       </c>
       <c r="D13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E13">
         <v>5.85</v>
@@ -1013,7 +1010,7 @@
         <v>40</v>
       </c>
       <c r="D14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E14">
         <v>22</v>
@@ -1030,7 +1027,7 @@
         <v>2.5</v>
       </c>
       <c r="D15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E15">
         <v>6</v>
@@ -1047,7 +1044,7 @@
         <v>90</v>
       </c>
       <c r="D16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E16">
         <v>3.75</v>
@@ -1064,7 +1061,7 @@
         <v>120</v>
       </c>
       <c r="D17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E17">
         <v>5.85</v>
@@ -1081,7 +1078,7 @@
         <v>50</v>
       </c>
       <c r="D18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E18">
         <v>22</v>
@@ -1098,7 +1095,7 @@
         <v>3.5</v>
       </c>
       <c r="D19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E19">
         <v>6</v>
@@ -1115,7 +1112,7 @@
         <v>45</v>
       </c>
       <c r="D20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E20">
         <v>3.75</v>
@@ -1132,7 +1129,7 @@
         <v>90</v>
       </c>
       <c r="D21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E21">
         <v>5.85</v>
@@ -1149,7 +1146,7 @@
         <v>30</v>
       </c>
       <c r="D22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E22">
         <v>10.5</v>
@@ -1166,7 +1163,7 @@
         <v>36</v>
       </c>
       <c r="D23" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E23">
         <v>7.8</v>
@@ -1183,7 +1180,7 @@
         <v>33</v>
       </c>
       <c r="D24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E24">
         <v>0.6</v>
@@ -1200,7 +1197,7 @@
         <v>90</v>
       </c>
       <c r="D25" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E25">
         <v>3.75</v>
@@ -1217,7 +1214,7 @@
         <v>120</v>
       </c>
       <c r="D26" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E26">
         <v>5.85</v>
@@ -1234,7 +1231,7 @@
         <v>45</v>
       </c>
       <c r="D27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E27">
         <v>10.5</v>
@@ -1251,7 +1248,7 @@
         <v>44</v>
       </c>
       <c r="D28" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E28">
         <v>7.8</v>
@@ -1268,7 +1265,7 @@
         <v>45</v>
       </c>
       <c r="D29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E29">
         <v>0.6</v>
@@ -1285,7 +1282,7 @@
         <v>45</v>
       </c>
       <c r="D30" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E30">
         <v>3.75</v>
@@ -1302,7 +1299,7 @@
         <v>90</v>
       </c>
       <c r="D31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E31">
         <v>5.85</v>
@@ -1319,7 +1316,7 @@
         <v>36</v>
       </c>
       <c r="D32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E32">
         <v>7.8</v>
@@ -1336,7 +1333,7 @@
         <v>16</v>
       </c>
       <c r="D33" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E33">
         <v>7.6</v>
@@ -1353,7 +1350,7 @@
         <v>70</v>
       </c>
       <c r="D34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E34">
         <v>1.2</v>
@@ -1370,7 +1367,7 @@
         <v>33</v>
       </c>
       <c r="D35" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E35">
         <v>0.6</v>
@@ -1387,7 +1384,7 @@
         <v>90</v>
       </c>
       <c r="D36" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E36">
         <v>3.75</v>
@@ -1404,7 +1401,7 @@
         <v>120</v>
       </c>
       <c r="D37" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E37">
         <v>5.85</v>
@@ -1421,7 +1418,7 @@
         <v>44</v>
       </c>
       <c r="D38" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E38">
         <v>7.8</v>
@@ -1438,7 +1435,7 @@
         <v>20</v>
       </c>
       <c r="D39" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E39">
         <v>7.6</v>
@@ -1455,7 +1452,7 @@
         <v>80</v>
       </c>
       <c r="D40" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E40">
         <v>1.2</v>
@@ -1472,7 +1469,7 @@
         <v>45</v>
       </c>
       <c r="D41" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E41">
         <v>0.6</v>
@@ -1489,7 +1486,7 @@
         <v>45</v>
       </c>
       <c r="D42" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E42">
         <v>3.75</v>
@@ -1506,7 +1503,7 @@
         <v>90</v>
       </c>
       <c r="D43" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E43">
         <v>5.85</v>
@@ -1523,7 +1520,7 @@
         <v>22</v>
       </c>
       <c r="D44" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E44">
         <v>8.35</v>
@@ -1540,7 +1537,7 @@
         <v>16</v>
       </c>
       <c r="D45" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E45">
         <v>7.6</v>
@@ -1557,7 +1554,7 @@
         <v>50</v>
       </c>
       <c r="D46" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E46">
         <v>12.75</v>
@@ -1574,7 +1571,7 @@
         <v>90</v>
       </c>
       <c r="D47" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E47">
         <v>3.75</v>
@@ -1591,7 +1588,7 @@
         <v>120</v>
       </c>
       <c r="D48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E48">
         <v>5.85</v>
@@ -1608,7 +1605,7 @@
         <v>35</v>
       </c>
       <c r="D49" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E49">
         <v>8.35</v>
@@ -1625,7 +1622,7 @@
         <v>20</v>
       </c>
       <c r="D50" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E50">
         <v>7.6</v>
@@ -1642,7 +1639,7 @@
         <v>60</v>
       </c>
       <c r="D51" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E51">
         <v>12.75</v>
@@ -1659,7 +1656,7 @@
         <v>45</v>
       </c>
       <c r="D52" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E52">
         <v>3.75</v>
@@ -1676,7 +1673,7 @@
         <v>90</v>
       </c>
       <c r="D53" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E53">
         <v>5.85</v>
@@ -1693,7 +1690,7 @@
         <v>60</v>
       </c>
       <c r="D54" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E54">
         <v>5.5</v>
@@ -1710,7 +1707,7 @@
         <v>16</v>
       </c>
       <c r="D55" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E55">
         <v>7.6</v>
@@ -1727,7 +1724,7 @@
         <v>43</v>
       </c>
       <c r="D56" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E56">
         <v>0.6</v>
@@ -1744,7 +1741,7 @@
         <v>90</v>
       </c>
       <c r="D57" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E57">
         <v>3.75</v>
@@ -1761,7 +1758,7 @@
         <v>120</v>
       </c>
       <c r="D58" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E58">
         <v>5.85</v>
@@ -1778,7 +1775,7 @@
         <v>78</v>
       </c>
       <c r="D59" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E59">
         <v>5.5</v>
@@ -1795,7 +1792,7 @@
         <v>20</v>
       </c>
       <c r="D60" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E60">
         <v>7.6</v>
@@ -1812,7 +1809,7 @@
         <v>55</v>
       </c>
       <c r="D61" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E61">
         <v>0.6</v>
@@ -1829,7 +1826,7 @@
         <v>45</v>
       </c>
       <c r="D62" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E62">
         <v>3.75</v>
@@ -1846,7 +1843,7 @@
         <v>90</v>
       </c>
       <c r="D63" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E63">
         <v>5.85</v>
@@ -1863,7 +1860,7 @@
         <v>14</v>
       </c>
       <c r="D64" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E64">
         <v>16.399999999999999</v>
@@ -1880,7 +1877,7 @@
         <v>78</v>
       </c>
       <c r="D65" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E65">
         <v>3</v>
@@ -1897,7 +1894,7 @@
         <v>20</v>
       </c>
       <c r="D66" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E66">
         <v>15.25</v>
@@ -1914,7 +1911,7 @@
         <v>90</v>
       </c>
       <c r="D67" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E67">
         <v>3.75</v>
@@ -1931,7 +1928,7 @@
         <v>120</v>
       </c>
       <c r="D68" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E68">
         <v>5.85</v>
@@ -1948,7 +1945,7 @@
         <v>18</v>
       </c>
       <c r="D69" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E69">
         <v>16.399999999999999</v>
@@ -1965,7 +1962,7 @@
         <v>90</v>
       </c>
       <c r="D70" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E70">
         <v>3</v>
@@ -1982,7 +1979,7 @@
         <v>35</v>
       </c>
       <c r="D71" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E71">
         <v>15.25</v>
@@ -1999,7 +1996,7 @@
         <v>22.5</v>
       </c>
       <c r="D72" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E72">
         <v>3.75</v>
@@ -2016,7 +2013,7 @@
         <v>40</v>
       </c>
       <c r="D73" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E73">
         <v>5.85</v>
@@ -2033,7 +2030,7 @@
         <v>35</v>
       </c>
       <c r="D74" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E74">
         <v>3</v>
@@ -2050,7 +2047,7 @@
         <v>30</v>
       </c>
       <c r="D75" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E75">
         <v>10.5</v>
@@ -2067,7 +2064,7 @@
         <v>40</v>
       </c>
       <c r="D76" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E76">
         <v>19.5</v>
@@ -2084,7 +2081,7 @@
         <v>40</v>
       </c>
       <c r="D77" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E77">
         <v>15</v>
@@ -2101,7 +2098,7 @@
         <v>55</v>
       </c>
       <c r="D78" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E78">
         <v>15</v>
@@ -2118,7 +2115,7 @@
         <v>40</v>
       </c>
       <c r="D79" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E79">
         <v>5.5</v>
@@ -2135,7 +2132,7 @@
         <v>20</v>
       </c>
       <c r="D80" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E80">
         <v>0.6</v>
@@ -2152,7 +2149,7 @@
         <v>20</v>
       </c>
       <c r="D81" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E81">
         <v>2</v>
@@ -2169,7 +2166,7 @@
         <v>15</v>
       </c>
       <c r="D82" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E82">
         <v>6.6</v>
@@ -2186,7 +2183,7 @@
         <v>15</v>
       </c>
       <c r="D83" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E83">
         <v>2.4</v>
@@ -2203,7 +2200,7 @@
         <v>20</v>
       </c>
       <c r="D84" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E84">
         <v>7.8</v>
@@ -2220,7 +2217,7 @@
         <v>25</v>
       </c>
       <c r="D85" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E85">
         <v>7.58</v>
@@ -2237,7 +2234,7 @@
         <v>20</v>
       </c>
       <c r="D86" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E86">
         <v>7.6</v>
@@ -2254,7 +2251,7 @@
         <v>20</v>
       </c>
       <c r="D87" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E87">
         <v>8.35</v>
@@ -2271,7 +2268,7 @@
         <v>25</v>
       </c>
       <c r="D88" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E88">
         <v>12.75</v>
@@ -2288,7 +2285,7 @@
         <v>20</v>
       </c>
       <c r="D89" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E89">
         <v>22</v>
@@ -2305,7 +2302,7 @@
         <v>4</v>
       </c>
       <c r="D90" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E90">
         <v>6.71</v>
@@ -2322,7 +2319,7 @@
         <v>30</v>
       </c>
       <c r="D91" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E91">
         <v>5</v>
@@ -2339,7 +2336,7 @@
         <v>25</v>
       </c>
       <c r="D92" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E92">
         <v>5.35</v>
@@ -2356,7 +2353,7 @@
         <v>40</v>
       </c>
       <c r="D93" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E93">
         <v>1.2</v>
@@ -2373,7 +2370,7 @@
         <v>45</v>
       </c>
       <c r="D94" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E94">
         <v>3</v>
@@ -2390,7 +2387,7 @@
         <v>50</v>
       </c>
       <c r="D95" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E95">
         <v>3.48</v>
@@ -2407,7 +2404,7 @@
         <v>30</v>
       </c>
       <c r="D96" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E96">
         <v>15.9</v>
@@ -2424,7 +2421,7 @@
         <v>20</v>
       </c>
       <c r="D97" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E97">
         <v>15.25</v>
@@ -2441,7 +2438,7 @@
         <v>35</v>
       </c>
       <c r="D98" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E98">
         <v>2.63</v>
@@ -2458,7 +2455,7 @@
         <v>40</v>
       </c>
       <c r="D99" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E99">
         <v>5.85</v>
@@ -2475,7 +2472,7 @@
         <v>35</v>
       </c>
       <c r="D100" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E100">
         <v>3</v>
@@ -2492,7 +2489,7 @@
         <v>30</v>
       </c>
       <c r="D101" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E101">
         <v>10.5</v>
@@ -2503,13 +2500,13 @@
         <v>20</v>
       </c>
       <c r="B102" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C102">
         <v>40</v>
       </c>
       <c r="D102" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E102">
         <v>19.5</v>
@@ -2526,7 +2523,7 @@
         <v>40</v>
       </c>
       <c r="D103" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E103">
         <v>15</v>
@@ -2543,7 +2540,7 @@
         <v>55</v>
       </c>
       <c r="D104" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E104">
         <v>15</v>
@@ -2560,7 +2557,7 @@
         <v>40</v>
       </c>
       <c r="D105" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E105">
         <v>5.5</v>
@@ -2577,7 +2574,7 @@
         <v>20</v>
       </c>
       <c r="D106" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E106">
         <v>0.6</v>
@@ -2594,7 +2591,7 @@
         <v>20</v>
       </c>
       <c r="D107" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E107">
         <v>2</v>
@@ -2611,7 +2608,7 @@
         <v>15</v>
       </c>
       <c r="D108" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E108">
         <v>6.6</v>
@@ -2628,7 +2625,7 @@
         <v>15</v>
       </c>
       <c r="D109" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E109">
         <v>2.4</v>
@@ -2645,7 +2642,7 @@
         <v>20</v>
       </c>
       <c r="D110" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E110">
         <v>7.8</v>
@@ -2662,7 +2659,7 @@
         <v>25</v>
       </c>
       <c r="D111" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E111">
         <v>7.58</v>
@@ -2679,7 +2676,7 @@
         <v>20</v>
       </c>
       <c r="D112" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E112">
         <v>7.6</v>
@@ -2696,7 +2693,7 @@
         <v>20</v>
       </c>
       <c r="D113" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E113">
         <v>8.35</v>
@@ -2713,7 +2710,7 @@
         <v>25</v>
       </c>
       <c r="D114" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E114">
         <v>12.75</v>
@@ -2730,7 +2727,7 @@
         <v>20</v>
       </c>
       <c r="D115" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E115">
         <v>22</v>
@@ -2747,7 +2744,7 @@
         <v>4</v>
       </c>
       <c r="D116" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E116">
         <v>4.83</v>
@@ -2764,7 +2761,7 @@
         <v>30</v>
       </c>
       <c r="D117" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E117">
         <v>5</v>
@@ -2781,7 +2778,7 @@
         <v>25</v>
       </c>
       <c r="D118" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E118">
         <v>5.35</v>
@@ -2798,7 +2795,7 @@
         <v>40</v>
       </c>
       <c r="D119" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E119">
         <v>1.2</v>
@@ -2815,7 +2812,7 @@
         <v>45</v>
       </c>
       <c r="D120" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E120">
         <v>3</v>
@@ -2832,7 +2829,7 @@
         <v>30</v>
       </c>
       <c r="D121" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E121">
         <v>15.9</v>
@@ -2849,7 +2846,7 @@
         <v>50</v>
       </c>
       <c r="D122" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E122">
         <v>3.48</v>
@@ -2866,7 +2863,7 @@
         <v>20</v>
       </c>
       <c r="D123" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E123">
         <v>15.25</v>
@@ -2883,7 +2880,7 @@
         <v>70</v>
       </c>
       <c r="D124" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E124">
         <v>2.63</v>
@@ -2900,7 +2897,7 @@
         <v>100</v>
       </c>
       <c r="D125" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E125">
         <v>5.85</v>
@@ -2917,7 +2914,7 @@
         <v>135</v>
       </c>
       <c r="D126" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E126">
         <v>2.63</v>
@@ -2934,7 +2931,7 @@
         <v>155</v>
       </c>
       <c r="D127" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E127">
         <v>5.85</v>
@@ -2951,7 +2948,7 @@
         <v>70</v>
       </c>
       <c r="D128" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E128">
         <v>2.63</v>
@@ -2968,7 +2965,7 @@
         <v>80</v>
       </c>
       <c r="D129" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E129">
         <v>5.85</v>
@@ -2985,7 +2982,7 @@
         <v>95</v>
       </c>
       <c r="D130" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E130">
         <v>3</v>
@@ -3002,7 +2999,7 @@
         <v>33</v>
       </c>
       <c r="D131" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E131">
         <v>10.5</v>
@@ -3019,7 +3016,7 @@
         <v>135</v>
       </c>
       <c r="D132" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E132">
         <v>2.63</v>
@@ -3036,7 +3033,7 @@
         <v>135</v>
       </c>
       <c r="D133" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E133">
         <v>5.85</v>
@@ -3053,7 +3050,7 @@
         <v>120</v>
       </c>
       <c r="D134" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E134">
         <v>3</v>
@@ -3070,7 +3067,7 @@
         <v>50</v>
       </c>
       <c r="D135" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E135">
         <v>10.5</v>
@@ -3087,7 +3084,7 @@
         <v>70</v>
       </c>
       <c r="D136" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E136">
         <v>2.63</v>
@@ -3098,13 +3095,13 @@
         <v>25</v>
       </c>
       <c r="B137" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C137">
         <v>5</v>
       </c>
       <c r="D137" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E137">
         <v>10.67</v>
@@ -3121,7 +3118,7 @@
         <v>100</v>
       </c>
       <c r="D138" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E138">
         <v>5.85</v>
@@ -3138,7 +3135,7 @@
         <v>80</v>
       </c>
       <c r="D139" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E139">
         <v>5</v>
@@ -3155,7 +3152,7 @@
         <v>135</v>
       </c>
       <c r="D140" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E140">
         <v>2.63</v>
@@ -3166,13 +3163,13 @@
         <v>26</v>
       </c>
       <c r="B141" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C141">
         <v>5</v>
       </c>
       <c r="D141" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E141">
         <v>10.67</v>
@@ -3189,7 +3186,7 @@
         <v>155</v>
       </c>
       <c r="D142" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E142">
         <v>5.85</v>
@@ -3206,7 +3203,7 @@
         <v>95</v>
       </c>
       <c r="D143" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E143">
         <v>5</v>
@@ -3223,7 +3220,7 @@
         <v>70</v>
       </c>
       <c r="D144" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E144">
         <v>2.63</v>
@@ -3240,7 +3237,7 @@
         <v>80</v>
       </c>
       <c r="D145" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E145">
         <v>5.85</v>
@@ -3257,7 +3254,7 @@
         <v>95</v>
       </c>
       <c r="D146" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E146">
         <v>3</v>
@@ -3274,7 +3271,7 @@
         <v>60</v>
       </c>
       <c r="D147" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E147">
         <v>5.5</v>
@@ -3291,7 +3288,7 @@
         <v>135</v>
       </c>
       <c r="D148" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E148">
         <v>2.63</v>
@@ -3308,7 +3305,7 @@
         <v>135</v>
       </c>
       <c r="D149" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E149">
         <v>5.85</v>
@@ -3325,7 +3322,7 @@
         <v>120</v>
       </c>
       <c r="D150" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E150">
         <v>3</v>
@@ -3342,7 +3339,7 @@
         <v>95</v>
       </c>
       <c r="D151" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E151">
         <v>5.5</v>
@@ -3359,7 +3356,7 @@
         <v>65</v>
       </c>
       <c r="D152" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E152">
         <v>5.85</v>
@@ -3376,7 +3373,7 @@
         <v>22</v>
       </c>
       <c r="D153" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E153">
         <v>8.35</v>
@@ -3393,7 +3390,7 @@
         <v>50</v>
       </c>
       <c r="D154" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E154">
         <v>12.75</v>
@@ -3410,7 +3407,7 @@
         <v>125</v>
       </c>
       <c r="D155" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E155">
         <v>5.85</v>
@@ -3427,7 +3424,7 @@
         <v>35</v>
       </c>
       <c r="D156" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E156">
         <v>8.35</v>
@@ -3444,7 +3441,7 @@
         <v>60</v>
       </c>
       <c r="D157" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E157">
         <v>12.75</v>
@@ -3461,7 +3458,7 @@
         <v>55</v>
       </c>
       <c r="D158" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E158">
         <v>2.63</v>
@@ -3478,7 +3475,7 @@
         <v>55</v>
       </c>
       <c r="D159" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E159">
         <v>5.85</v>
@@ -3489,13 +3486,13 @@
         <v>31</v>
       </c>
       <c r="B160" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C160">
         <v>36</v>
       </c>
       <c r="D160" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E160">
         <v>10.5</v>
@@ -3512,7 +3509,7 @@
         <v>50</v>
       </c>
       <c r="D161" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E161">
         <v>3.48</v>
@@ -3529,7 +3526,7 @@
         <v>70</v>
       </c>
       <c r="D162" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E162">
         <v>2.63</v>
@@ -3546,7 +3543,7 @@
         <v>65</v>
       </c>
       <c r="D163" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E163">
         <v>5.85</v>
@@ -3563,7 +3560,7 @@
         <v>65</v>
       </c>
       <c r="D164" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E164">
         <v>15</v>
@@ -3580,7 +3577,7 @@
         <v>33</v>
       </c>
       <c r="D165" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E165">
         <v>2</v>
@@ -3597,7 +3594,7 @@
         <v>33</v>
       </c>
       <c r="D166" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E166">
         <v>0.6</v>
@@ -3614,7 +3611,7 @@
         <v>135</v>
       </c>
       <c r="D167" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E167">
         <v>2.63</v>
@@ -3631,7 +3628,7 @@
         <v>125</v>
       </c>
       <c r="D168" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E168">
         <v>5.85</v>
@@ -3648,7 +3645,7 @@
         <v>95</v>
       </c>
       <c r="D169" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E169">
         <v>15</v>
@@ -3665,7 +3662,7 @@
         <v>40</v>
       </c>
       <c r="D170" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E170">
         <v>2</v>
@@ -3682,7 +3679,7 @@
         <v>41</v>
       </c>
       <c r="D171" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E171">
         <v>0.6</v>
@@ -3699,7 +3696,7 @@
         <v>70</v>
       </c>
       <c r="D172" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E172">
         <v>2.63</v>
@@ -3716,7 +3713,7 @@
         <v>55</v>
       </c>
       <c r="D173" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E173">
         <v>5.85</v>
@@ -3733,7 +3730,7 @@
         <v>65</v>
       </c>
       <c r="D174" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E174">
         <v>15</v>
@@ -3750,7 +3747,7 @@
         <v>70</v>
       </c>
       <c r="D175" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E175">
         <v>19.5</v>
@@ -3767,7 +3764,7 @@
         <v>60</v>
       </c>
       <c r="D176" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E176">
         <v>15</v>
@@ -3784,7 +3781,7 @@
         <v>33</v>
       </c>
       <c r="D177" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E177">
         <v>0.6</v>
@@ -3801,7 +3798,7 @@
         <v>135</v>
       </c>
       <c r="D178" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E178">
         <v>2.63</v>
@@ -3818,7 +3815,7 @@
         <v>100</v>
       </c>
       <c r="D179" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E179">
         <v>5.85</v>
@@ -3835,7 +3832,7 @@
         <v>95</v>
       </c>
       <c r="D180" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E180">
         <v>15</v>
@@ -3852,7 +3849,7 @@
         <v>85</v>
       </c>
       <c r="D181" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E181">
         <v>19.5</v>
@@ -3869,7 +3866,7 @@
         <v>80</v>
       </c>
       <c r="D182" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E182">
         <v>15</v>
@@ -3886,7 +3883,7 @@
         <v>45</v>
       </c>
       <c r="D183" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E183">
         <v>0.6</v>
@@ -3903,7 +3900,7 @@
         <v>70</v>
       </c>
       <c r="D184" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E184">
         <v>2.63</v>
@@ -3920,7 +3917,7 @@
         <v>65</v>
       </c>
       <c r="D185" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E185">
         <v>5.85</v>
@@ -3937,7 +3934,7 @@
         <v>50</v>
       </c>
       <c r="D186" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E186">
         <v>7.8</v>
@@ -3954,7 +3951,7 @@
         <v>45</v>
       </c>
       <c r="D187" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E187">
         <v>0.6</v>
@@ -3971,7 +3968,7 @@
         <v>50</v>
       </c>
       <c r="D188" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E188">
         <v>3.48</v>
@@ -3988,7 +3985,7 @@
         <v>135</v>
       </c>
       <c r="D189" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E189">
         <v>2.63</v>
@@ -4005,7 +4002,7 @@
         <v>125</v>
       </c>
       <c r="D190" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E190">
         <v>5.85</v>
@@ -4022,7 +4019,7 @@
         <v>120</v>
       </c>
       <c r="D191" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E191">
         <v>7.8</v>
@@ -4039,7 +4036,7 @@
         <v>55</v>
       </c>
       <c r="D192" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E192">
         <v>0.6</v>
@@ -4056,7 +4053,7 @@
         <v>100</v>
       </c>
       <c r="D193" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E193">
         <v>3.48</v>
@@ -4073,7 +4070,7 @@
         <v>70</v>
       </c>
       <c r="D194" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E194">
         <v>2.63</v>
@@ -4090,7 +4087,7 @@
         <v>100</v>
       </c>
       <c r="D195" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E195">
         <v>5.85</v>
@@ -4107,7 +4104,7 @@
         <v>70</v>
       </c>
       <c r="D196" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E196">
         <v>3</v>
@@ -4124,7 +4121,7 @@
         <v>40</v>
       </c>
       <c r="D197" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E197">
         <v>15.25</v>
@@ -4141,7 +4138,7 @@
         <v>135</v>
       </c>
       <c r="D198" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E198">
         <v>2.63</v>
@@ -4158,7 +4155,7 @@
         <v>155</v>
       </c>
       <c r="D199" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E199">
         <v>5.85</v>
@@ -4175,7 +4172,7 @@
         <v>105</v>
       </c>
       <c r="D200" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E200">
         <v>3</v>
@@ -4192,7 +4189,7 @@
         <v>35</v>
       </c>
       <c r="D201" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E201">
         <v>15.25</v>
@@ -4209,7 +4206,7 @@
         <v>70</v>
       </c>
       <c r="D202" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E202">
         <v>2.63</v>
@@ -4226,7 +4223,7 @@
         <v>65</v>
       </c>
       <c r="D203" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E203">
         <v>5.85</v>
@@ -4243,7 +4240,7 @@
         <v>50</v>
       </c>
       <c r="D204" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E204">
         <v>12.75</v>
@@ -4254,13 +4251,13 @@
         <v>40</v>
       </c>
       <c r="B205" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C205">
         <v>12</v>
       </c>
       <c r="D205" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E205">
         <v>5.35</v>
@@ -4277,7 +4274,7 @@
         <v>135</v>
       </c>
       <c r="D206" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E206">
         <v>2.63</v>
@@ -4294,7 +4291,7 @@
         <v>125</v>
       </c>
       <c r="D207" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E207">
         <v>5.85</v>
@@ -4311,7 +4308,7 @@
         <v>60</v>
       </c>
       <c r="D208" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E208">
         <v>12.75</v>
@@ -4322,13 +4319,13 @@
         <v>41</v>
       </c>
       <c r="B209" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C209">
         <v>18</v>
       </c>
       <c r="D209" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E209">
         <v>5.35</v>
@@ -4345,7 +4342,7 @@
         <v>70</v>
       </c>
       <c r="D210" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E210">
         <v>2.63</v>
@@ -4362,7 +4359,7 @@
         <v>65</v>
       </c>
       <c r="D211" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E211">
         <v>5.85</v>
@@ -4379,7 +4376,7 @@
         <v>70</v>
       </c>
       <c r="D212" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E212">
         <v>19.5</v>
@@ -4396,7 +4393,7 @@
         <v>30</v>
       </c>
       <c r="D213" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E213">
         <v>10.5</v>
@@ -4413,7 +4410,7 @@
         <v>33</v>
       </c>
       <c r="D214" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E214">
         <v>0.6</v>
@@ -4430,7 +4427,7 @@
         <v>135</v>
       </c>
       <c r="D215" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E215">
         <v>2.63</v>
@@ -4447,7 +4444,7 @@
         <v>125</v>
       </c>
       <c r="D216" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E216">
         <v>5.85</v>
@@ -4464,7 +4461,7 @@
         <v>85</v>
       </c>
       <c r="D217" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E217">
         <v>19.5</v>
@@ -4481,7 +4478,7 @@
         <v>40</v>
       </c>
       <c r="D218" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E218">
         <v>10.5</v>
@@ -4498,7 +4495,7 @@
         <v>45</v>
       </c>
       <c r="D219" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E219">
         <v>0.6</v>
@@ -4515,7 +4512,7 @@
         <v>70</v>
       </c>
       <c r="D220" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E220">
         <v>2.63</v>
@@ -4532,7 +4529,7 @@
         <v>65</v>
       </c>
       <c r="D221" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E221">
         <v>5.85</v>
@@ -4549,7 +4546,7 @@
         <v>65</v>
       </c>
       <c r="D222" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E222">
         <v>15</v>
@@ -4566,7 +4563,7 @@
         <v>13</v>
       </c>
       <c r="D223" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E223">
         <v>2.4</v>
@@ -4583,7 +4580,7 @@
         <v>60</v>
       </c>
       <c r="D224" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E224">
         <v>15</v>
@@ -4600,7 +4597,7 @@
         <v>135</v>
       </c>
       <c r="D225" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E225">
         <v>2.63</v>
@@ -4617,7 +4614,7 @@
         <v>125</v>
       </c>
       <c r="D226" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E226">
         <v>5.85</v>
@@ -4634,7 +4631,7 @@
         <v>95</v>
       </c>
       <c r="D227" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E227">
         <v>15</v>
@@ -4651,7 +4648,7 @@
         <v>20</v>
       </c>
       <c r="D228" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E228">
         <v>2.4</v>
@@ -4668,7 +4665,7 @@
         <v>80</v>
       </c>
       <c r="D229" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E229">
         <v>15</v>
@@ -4685,7 +4682,7 @@
         <v>70</v>
       </c>
       <c r="D230" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E230">
         <v>2.63</v>
@@ -4702,7 +4699,7 @@
         <v>55</v>
       </c>
       <c r="D231" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E231">
         <v>5.85</v>
@@ -4713,13 +4710,13 @@
         <v>46</v>
       </c>
       <c r="B232" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C232">
         <v>25</v>
       </c>
       <c r="D232" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E232">
         <v>10.5</v>
@@ -4736,7 +4733,7 @@
         <v>44</v>
       </c>
       <c r="D233" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E233">
         <v>7.58</v>
@@ -4753,7 +4750,7 @@
         <v>65</v>
       </c>
       <c r="D234" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E234">
         <v>3</v>
@@ -4770,7 +4767,7 @@
         <v>25</v>
       </c>
       <c r="D235" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E235">
         <v>2</v>
@@ -4787,7 +4784,7 @@
         <v>16</v>
       </c>
       <c r="D236" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E236">
         <v>6.6</v>
@@ -4804,7 +4801,7 @@
         <v>135</v>
       </c>
       <c r="D237" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E237">
         <v>2.63</v>
@@ -4821,7 +4818,7 @@
         <v>89</v>
       </c>
       <c r="D238" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E238">
         <v>5.85</v>
@@ -4832,13 +4829,13 @@
         <v>47</v>
       </c>
       <c r="B239" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C239">
         <v>35</v>
       </c>
       <c r="D239" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E239">
         <v>10.5</v>
@@ -4855,7 +4852,7 @@
         <v>60</v>
       </c>
       <c r="D240" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E240">
         <v>7.58</v>
@@ -4872,7 +4869,7 @@
         <v>100</v>
       </c>
       <c r="D241" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E241">
         <v>3</v>
@@ -4889,7 +4886,7 @@
         <v>35</v>
       </c>
       <c r="D242" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E242">
         <v>2</v>
@@ -4906,7 +4903,7 @@
         <v>20</v>
       </c>
       <c r="D243" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E243">
         <v>6.6</v>
@@ -4923,7 +4920,7 @@
         <v>70</v>
       </c>
       <c r="D244" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E244">
         <v>2.63</v>
@@ -4940,7 +4937,7 @@
         <v>65</v>
       </c>
       <c r="D245" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E245">
         <v>5.85</v>
@@ -4957,7 +4954,7 @@
         <v>40</v>
       </c>
       <c r="D246" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E246">
         <v>5</v>
@@ -4974,7 +4971,7 @@
         <v>30</v>
       </c>
       <c r="D247" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E247">
         <v>5.35</v>
@@ -4991,7 +4988,7 @@
         <v>3</v>
       </c>
       <c r="D248" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E248">
         <v>6.71</v>
@@ -5008,7 +5005,7 @@
         <v>33</v>
       </c>
       <c r="D249" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E249">
         <v>0.6</v>
@@ -5025,7 +5022,7 @@
         <v>135</v>
       </c>
       <c r="D250" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E250">
         <v>2.63</v>
@@ -5042,7 +5039,7 @@
         <v>125</v>
       </c>
       <c r="D251" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E251">
         <v>5.85</v>
@@ -5059,7 +5056,7 @@
         <v>60</v>
       </c>
       <c r="D252" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E252">
         <v>5</v>
@@ -5076,7 +5073,7 @@
         <v>40</v>
       </c>
       <c r="D253" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E253">
         <v>5.35</v>
@@ -5093,7 +5090,7 @@
         <v>5</v>
       </c>
       <c r="D254" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E254">
         <v>6.71</v>
@@ -5110,7 +5107,7 @@
         <v>45</v>
       </c>
       <c r="D255" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E255">
         <v>0.6</v>
@@ -5127,7 +5124,7 @@
         <v>70</v>
       </c>
       <c r="D256" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E256">
         <v>2.63</v>
@@ -5144,7 +5141,7 @@
         <v>55</v>
       </c>
       <c r="D257" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E257">
         <v>5.85</v>
@@ -5161,7 +5158,7 @@
         <v>65</v>
       </c>
       <c r="D258" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E258">
         <v>3</v>
@@ -5178,7 +5175,7 @@
         <v>16</v>
       </c>
       <c r="D259" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E259">
         <v>6.6</v>
@@ -5195,7 +5192,7 @@
         <v>25</v>
       </c>
       <c r="D260" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E260">
         <v>2</v>
@@ -5212,7 +5209,7 @@
         <v>25</v>
       </c>
       <c r="D261" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E261">
         <v>0.6</v>
@@ -5229,7 +5226,7 @@
         <v>135</v>
       </c>
       <c r="D262" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E262">
         <v>2.63</v>
@@ -5246,7 +5243,7 @@
         <v>89</v>
       </c>
       <c r="D263" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E263">
         <v>5.85</v>
@@ -5263,7 +5260,7 @@
         <v>100</v>
       </c>
       <c r="D264" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E264">
         <v>3</v>
@@ -5280,7 +5277,7 @@
         <v>20</v>
       </c>
       <c r="D265" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E265">
         <v>6.6</v>
@@ -5297,7 +5294,7 @@
         <v>35</v>
       </c>
       <c r="D266" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E266">
         <v>2</v>
@@ -5314,7 +5311,7 @@
         <v>35</v>
       </c>
       <c r="D267" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E267">
         <v>0.6</v>
@@ -5325,13 +5322,13 @@
         <v>53</v>
       </c>
       <c r="B268" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C268">
         <v>4</v>
       </c>
       <c r="D268" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E268">
         <v>23.7</v>
@@ -5342,13 +5339,13 @@
         <v>53</v>
       </c>
       <c r="B269" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C269">
         <v>4</v>
       </c>
       <c r="D269" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E269">
         <v>4</v>
@@ -5359,13 +5356,13 @@
         <v>53</v>
       </c>
       <c r="B270" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C270">
         <v>20</v>
       </c>
       <c r="D270" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E270">
         <v>5.85</v>
@@ -5376,13 +5373,13 @@
         <v>54</v>
       </c>
       <c r="B271" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C271">
         <v>4</v>
       </c>
       <c r="D271" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E271">
         <v>23.7</v>
@@ -5393,13 +5390,13 @@
         <v>54</v>
       </c>
       <c r="B272" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C272">
         <v>4</v>
       </c>
       <c r="D272" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E272">
         <v>4</v>
@@ -5410,13 +5407,13 @@
         <v>55</v>
       </c>
       <c r="B273" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C273">
         <v>50</v>
       </c>
       <c r="D273" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E273">
         <v>6</v>
@@ -5427,13 +5424,13 @@
         <v>55</v>
       </c>
       <c r="B274" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C274">
         <v>20</v>
       </c>
       <c r="D274" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E274">
         <v>1.4</v>
@@ -5450,7 +5447,7 @@
         <v>105</v>
       </c>
       <c r="D275" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E275">
         <v>5.5</v>
@@ -5461,13 +5458,13 @@
         <v>55</v>
       </c>
       <c r="B276" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C276">
         <v>12</v>
       </c>
       <c r="D276" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E276">
         <v>13.5</v>
@@ -5484,7 +5481,7 @@
         <v>45</v>
       </c>
       <c r="D277" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E277">
         <v>5</v>
@@ -5501,7 +5498,7 @@
         <v>23</v>
       </c>
       <c r="D278" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E278">
         <v>15.25</v>
@@ -5512,13 +5509,13 @@
         <v>55</v>
       </c>
       <c r="B279" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C279">
         <v>12</v>
       </c>
       <c r="D279" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E279">
         <v>6.9</v>
@@ -5529,13 +5526,13 @@
         <v>55</v>
       </c>
       <c r="B280" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C280">
         <v>7</v>
       </c>
       <c r="D280" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E280">
         <v>4.5</v>
@@ -5546,13 +5543,13 @@
         <v>56</v>
       </c>
       <c r="B281" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C281">
         <v>50</v>
       </c>
       <c r="D281" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E281">
         <v>6</v>
@@ -5563,13 +5560,13 @@
         <v>56</v>
       </c>
       <c r="B282" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C282">
         <v>20</v>
       </c>
       <c r="D282" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E282">
         <v>1.4</v>
@@ -5586,7 +5583,7 @@
         <v>110</v>
       </c>
       <c r="D283" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E283">
         <v>7.58</v>
@@ -5597,13 +5594,13 @@
         <v>56</v>
       </c>
       <c r="B284" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C284">
         <v>12</v>
       </c>
       <c r="D284" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E284">
         <v>13.5</v>
@@ -5620,7 +5617,7 @@
         <v>45</v>
       </c>
       <c r="D285" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E285">
         <v>5</v>
@@ -5637,7 +5634,7 @@
         <v>23</v>
       </c>
       <c r="D286" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E286">
         <v>15.25</v>
@@ -5648,13 +5645,13 @@
         <v>56</v>
       </c>
       <c r="B287" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C287">
         <v>12</v>
       </c>
       <c r="D287" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E287">
         <v>6.9</v>
@@ -5665,13 +5662,13 @@
         <v>56</v>
       </c>
       <c r="B288" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C288">
         <v>7</v>
       </c>
       <c r="D288" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E288">
         <v>4.5</v>
@@ -5682,13 +5679,13 @@
         <v>57</v>
       </c>
       <c r="B289" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C289">
         <v>50</v>
       </c>
       <c r="D289" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E289">
         <v>6</v>
@@ -5699,13 +5696,13 @@
         <v>57</v>
       </c>
       <c r="B290" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C290">
         <v>20</v>
       </c>
       <c r="D290" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E290">
         <v>1.4</v>
@@ -5722,7 +5719,7 @@
         <v>60</v>
       </c>
       <c r="D291" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E291">
         <v>12.75</v>
@@ -5733,13 +5730,13 @@
         <v>57</v>
       </c>
       <c r="B292" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C292">
         <v>12</v>
       </c>
       <c r="D292" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E292">
         <v>13.5</v>
@@ -5756,7 +5753,7 @@
         <v>45</v>
       </c>
       <c r="D293" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E293">
         <v>5</v>
@@ -5773,7 +5770,7 @@
         <v>23</v>
       </c>
       <c r="D294" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E294">
         <v>15.25</v>
@@ -5784,13 +5781,13 @@
         <v>57</v>
       </c>
       <c r="B295" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C295">
         <v>12</v>
       </c>
       <c r="D295" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E295">
         <v>6.9</v>
@@ -5801,13 +5798,13 @@
         <v>57</v>
       </c>
       <c r="B296" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C296">
         <v>7</v>
       </c>
       <c r="D296" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E296">
         <v>4.5</v>
@@ -5818,13 +5815,13 @@
         <v>58</v>
       </c>
       <c r="B297" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C297">
         <v>125</v>
       </c>
       <c r="D297" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E297">
         <v>9.9</v>
@@ -5835,13 +5832,13 @@
         <v>58</v>
       </c>
       <c r="B298" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C298">
         <v>20</v>
       </c>
       <c r="D298" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E298">
         <v>1.4</v>
@@ -5852,13 +5849,13 @@
         <v>58</v>
       </c>
       <c r="B299" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C299">
         <v>50</v>
       </c>
       <c r="D299" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E299">
         <v>6</v>
@@ -5869,13 +5866,13 @@
         <v>58</v>
       </c>
       <c r="B300" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C300">
         <v>52</v>
       </c>
       <c r="D300" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E300">
         <v>15.9</v>
@@ -5892,7 +5889,7 @@
         <v>23</v>
       </c>
       <c r="D301" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E301">
         <v>15.25</v>
@@ -5903,13 +5900,13 @@
         <v>58</v>
       </c>
       <c r="B302" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C302">
         <v>7</v>
       </c>
       <c r="D302" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E302">
         <v>4.5</v>
@@ -5926,7 +5923,7 @@
         <v>45</v>
       </c>
       <c r="D303" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E303">
         <v>5</v>
@@ -5937,13 +5934,13 @@
         <v>58</v>
       </c>
       <c r="B304" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C304">
         <v>12</v>
       </c>
       <c r="D304" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E304">
         <v>13.5</v>
@@ -5954,13 +5951,13 @@
         <v>58</v>
       </c>
       <c r="B305" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C305">
         <v>12</v>
       </c>
       <c r="D305" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E305">
         <v>6.9</v>
@@ -5968,16 +5965,16 @@
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B306" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C306">
         <v>125</v>
       </c>
       <c r="D306" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E306">
         <v>9.9</v>
@@ -5985,16 +5982,16 @@
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B307" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C307">
         <v>12</v>
       </c>
       <c r="D307" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E307">
         <v>13.5</v>
@@ -6002,7 +5999,7 @@
     </row>
     <row r="308" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B308" t="s">
         <v>87</v>
@@ -6011,7 +6008,7 @@
         <v>45</v>
       </c>
       <c r="D308" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E308">
         <v>5</v>
@@ -6019,16 +6016,16 @@
     </row>
     <row r="309" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B309" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C309">
         <v>7</v>
       </c>
       <c r="D309" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E309">
         <v>4.5</v>
@@ -6036,16 +6033,16 @@
     </row>
     <row r="310" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B310" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C310">
         <v>12</v>
       </c>
       <c r="D310" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E310">
         <v>6.9</v>
@@ -6056,13 +6053,13 @@
         <v>59</v>
       </c>
       <c r="B311" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C311">
         <v>140</v>
       </c>
       <c r="D311" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E311">
         <v>9.9</v>
@@ -6073,13 +6070,13 @@
         <v>59</v>
       </c>
       <c r="B312" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C312">
         <v>50</v>
       </c>
       <c r="D312" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E312">
         <v>6</v>
@@ -6096,7 +6093,7 @@
         <v>62</v>
       </c>
       <c r="D313" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E313">
         <v>22</v>
@@ -6113,7 +6110,7 @@
         <v>23</v>
       </c>
       <c r="D314" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E314">
         <v>15.25</v>
@@ -6124,13 +6121,13 @@
         <v>59</v>
       </c>
       <c r="B315" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C315">
         <v>7</v>
       </c>
       <c r="D315" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E315">
         <v>4.5</v>
@@ -6147,7 +6144,7 @@
         <v>45</v>
       </c>
       <c r="D316" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E316">
         <v>5</v>
@@ -6158,13 +6155,13 @@
         <v>59</v>
       </c>
       <c r="B317" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C317">
         <v>12</v>
       </c>
       <c r="D317" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E317">
         <v>13.5</v>
@@ -6175,13 +6172,13 @@
         <v>59</v>
       </c>
       <c r="B318" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C318">
         <v>20</v>
       </c>
       <c r="D318" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E318">
         <v>1.4</v>
@@ -6192,13 +6189,13 @@
         <v>59</v>
       </c>
       <c r="B319" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C319">
         <v>12</v>
       </c>
       <c r="D319" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E319">
         <v>6.9</v>
@@ -6209,13 +6206,13 @@
         <v>60</v>
       </c>
       <c r="B320" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C320">
         <v>125</v>
       </c>
       <c r="D320" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E320">
         <v>9.9</v>
@@ -6226,13 +6223,13 @@
         <v>60</v>
       </c>
       <c r="B321" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C321">
         <v>20</v>
       </c>
       <c r="D321" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E321">
         <v>1.4</v>
@@ -6243,13 +6240,13 @@
         <v>60</v>
       </c>
       <c r="B322" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C322">
         <v>50</v>
       </c>
       <c r="D322" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E322">
         <v>6</v>
@@ -6266,7 +6263,7 @@
         <v>62</v>
       </c>
       <c r="D323" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E323">
         <v>22</v>
@@ -6283,7 +6280,7 @@
         <v>23</v>
       </c>
       <c r="D324" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E324">
         <v>15.25</v>
@@ -6294,13 +6291,13 @@
         <v>60</v>
       </c>
       <c r="B325" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C325">
         <v>7</v>
       </c>
       <c r="D325" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E325">
         <v>4.5</v>
@@ -6317,7 +6314,7 @@
         <v>45</v>
       </c>
       <c r="D326" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E326">
         <v>5</v>
@@ -6328,13 +6325,13 @@
         <v>60</v>
       </c>
       <c r="B327" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C327">
         <v>12</v>
       </c>
       <c r="D327" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E327">
         <v>13.5</v>
@@ -6345,13 +6342,13 @@
         <v>60</v>
       </c>
       <c r="B328" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C328">
         <v>12</v>
       </c>
       <c r="D328" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E328">
         <v>6.9</v>
@@ -6362,13 +6359,13 @@
         <v>61</v>
       </c>
       <c r="B329" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C329">
         <v>125</v>
       </c>
       <c r="D329" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E329">
         <v>9.9</v>
@@ -6379,13 +6376,13 @@
         <v>61</v>
       </c>
       <c r="B330" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C330">
         <v>50</v>
       </c>
       <c r="D330" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E330">
         <v>6</v>
@@ -6396,13 +6393,13 @@
         <v>61</v>
       </c>
       <c r="B331" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C331">
         <v>52</v>
       </c>
       <c r="D331" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E331">
         <v>15.9</v>
@@ -6419,7 +6416,7 @@
         <v>23</v>
       </c>
       <c r="D332" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E332">
         <v>15.25</v>
@@ -6430,13 +6427,13 @@
         <v>61</v>
       </c>
       <c r="B333" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C333">
         <v>7</v>
       </c>
       <c r="D333" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E333">
         <v>4.5</v>
@@ -6447,13 +6444,13 @@
         <v>61</v>
       </c>
       <c r="B334" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C334">
         <v>12</v>
       </c>
       <c r="D334" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E334">
         <v>6.9</v>
@@ -6464,13 +6461,13 @@
         <v>61</v>
       </c>
       <c r="B335" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C335">
         <v>20</v>
       </c>
       <c r="D335" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E335">
         <v>1.4</v>
@@ -6478,7 +6475,7 @@
     </row>
     <row r="336" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B336" t="s">
         <v>87</v>
@@ -6487,7 +6484,7 @@
         <v>45</v>
       </c>
       <c r="D336" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E336">
         <v>5</v>
@@ -6495,16 +6492,16 @@
     </row>
     <row r="337" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B337" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C337">
         <v>7</v>
       </c>
       <c r="D337" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E337">
         <v>4.5</v>
@@ -6512,16 +6509,16 @@
     </row>
     <row r="338" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B338" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C338">
         <v>12</v>
       </c>
       <c r="D338" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E338">
         <v>6.9</v>
@@ -6529,7 +6526,7 @@
     </row>
     <row r="339" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B339" t="s">
         <v>77</v>
@@ -6538,7 +6535,7 @@
         <v>23</v>
       </c>
       <c r="D339" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E339">
         <v>15.25</v>
@@ -6546,16 +6543,16 @@
     </row>
     <row r="340" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B340" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C340">
         <v>12</v>
       </c>
       <c r="D340" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E340">
         <v>13.5</v>
@@ -6563,7 +6560,7 @@
     </row>
     <row r="341" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B341" t="s">
         <v>77</v>
@@ -6572,7 +6569,7 @@
         <v>23</v>
       </c>
       <c r="D341" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E341">
         <v>15.25</v>
@@ -6580,16 +6577,16 @@
     </row>
     <row r="342" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B342" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C342">
         <v>12</v>
       </c>
       <c r="D342" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E342">
         <v>6.9</v>
@@ -6597,16 +6594,16 @@
     </row>
     <row r="343" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B343" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C343">
         <v>7</v>
       </c>
       <c r="D343" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E343">
         <v>4.5</v>
@@ -6614,16 +6611,16 @@
     </row>
     <row r="344" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B344" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C344">
         <v>20</v>
       </c>
       <c r="D344" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E344">
         <v>1.4</v>
@@ -6631,7 +6628,7 @@
     </row>
     <row r="345" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B345" t="s">
         <v>87</v>
@@ -6640,7 +6637,7 @@
         <v>45</v>
       </c>
       <c r="D345" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E345">
         <v>5</v>
@@ -6648,16 +6645,16 @@
     </row>
     <row r="346" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B346" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C346">
         <v>50</v>
       </c>
       <c r="D346" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E346">
         <v>6</v>
@@ -6665,7 +6662,7 @@
     </row>
     <row r="347" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B347" t="s">
         <v>85</v>
@@ -6674,7 +6671,7 @@
         <v>110</v>
       </c>
       <c r="D347" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E347">
         <v>7.58</v>
@@ -6685,13 +6682,13 @@
         <v>61</v>
       </c>
       <c r="B348" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C348">
         <v>12</v>
       </c>
       <c r="D348" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E348">
         <v>13.5</v>
@@ -6699,7 +6696,7 @@
     </row>
     <row r="349" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B349" t="s">
         <v>91</v>
@@ -6708,7 +6705,7 @@
         <v>205</v>
       </c>
       <c r="D349" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E349">
         <v>2.63</v>
@@ -6716,7 +6713,7 @@
     </row>
     <row r="350" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B350" t="s">
         <v>79</v>
@@ -6725,7 +6722,7 @@
         <v>75</v>
       </c>
       <c r="D350" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E350">
         <v>15</v>
@@ -6733,7 +6730,7 @@
     </row>
     <row r="351" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B351" t="s">
         <v>87</v>
@@ -6742,7 +6739,7 @@
         <v>44</v>
       </c>
       <c r="D351" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E351">
         <v>5</v>
@@ -6750,7 +6747,7 @@
     </row>
     <row r="352" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B352" t="s">
         <v>77</v>
@@ -6759,7 +6756,7 @@
         <v>10</v>
       </c>
       <c r="D352" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E352">
         <v>15.25</v>
@@ -6767,16 +6764,16 @@
     </row>
     <row r="353" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B353" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C353">
         <v>210</v>
       </c>
       <c r="D353" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E353">
         <v>2.4500000000000002</v>
@@ -6784,16 +6781,16 @@
     </row>
     <row r="354" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
+        <v>107</v>
+      </c>
+      <c r="B354" t="s">
         <v>108</v>
-      </c>
-      <c r="B354" t="s">
-        <v>109</v>
       </c>
       <c r="C354">
         <v>220</v>
       </c>
       <c r="D354" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E354">
         <v>3.3</v>
@@ -6801,7 +6798,7 @@
     </row>
     <row r="355" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B355" t="s">
         <v>76</v>
@@ -6810,7 +6807,7 @@
         <v>40</v>
       </c>
       <c r="D355" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E355">
         <v>3.3</v>
@@ -6818,16 +6815,16 @@
     </row>
     <row r="356" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A356" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B356" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C356">
         <v>25</v>
       </c>
       <c r="D356" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E356">
         <v>16.399999999999999</v>
@@ -6835,7 +6832,7 @@
     </row>
     <row r="357" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B357" t="s">
         <v>77</v>
@@ -6844,7 +6841,7 @@
         <v>10</v>
       </c>
       <c r="D357" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E357">
         <v>15.25</v>
@@ -6852,16 +6849,16 @@
     </row>
     <row r="358" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B358" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C358">
         <v>210</v>
       </c>
       <c r="D358" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E358">
         <v>2.4500000000000002</v>
@@ -6872,13 +6869,13 @@
         <v>67</v>
       </c>
       <c r="B359" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C359">
         <v>220</v>
       </c>
       <c r="D359" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E359">
         <v>3.3</v>
@@ -6895,7 +6892,7 @@
         <v>60</v>
       </c>
       <c r="D360" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E360">
         <v>22</v>
@@ -6912,7 +6909,7 @@
         <v>10</v>
       </c>
       <c r="D361" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E361">
         <v>15.25</v>
@@ -6923,13 +6920,13 @@
         <v>67</v>
       </c>
       <c r="B362" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C362">
         <v>230</v>
       </c>
       <c r="D362" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E362">
         <v>2.4500000000000002</v>
@@ -6937,16 +6934,16 @@
     </row>
     <row r="363" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A363" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B363" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C363">
         <v>220</v>
       </c>
       <c r="D363" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E363">
         <v>3.3</v>
@@ -6954,7 +6951,7 @@
     </row>
     <row r="364" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A364" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B364" t="s">
         <v>70</v>
@@ -6963,7 +6960,7 @@
         <v>45</v>
       </c>
       <c r="D364" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E364">
         <v>7.8</v>
@@ -6971,7 +6968,7 @@
     </row>
     <row r="365" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A365" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B365" t="s">
         <v>77</v>
@@ -6980,7 +6977,7 @@
         <v>10</v>
       </c>
       <c r="D365" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E365">
         <v>15.25</v>
@@ -6988,16 +6985,16 @@
     </row>
     <row r="366" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A366" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B366" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C366">
         <v>230</v>
       </c>
       <c r="D366" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E366">
         <v>2.4500000000000002</v>
@@ -7005,16 +7002,16 @@
     </row>
     <row r="367" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A367" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B367" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C367">
         <v>220</v>
       </c>
       <c r="D367" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E367">
         <v>3.3</v>
@@ -7022,7 +7019,7 @@
     </row>
     <row r="368" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A368" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B368" t="s">
         <v>74</v>
@@ -7031,7 +7028,7 @@
         <v>78</v>
       </c>
       <c r="D368" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E368">
         <v>5.5</v>
@@ -7039,7 +7036,7 @@
     </row>
     <row r="369" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A369" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B369" t="s">
         <v>76</v>
@@ -7048,7 +7045,7 @@
         <v>40</v>
       </c>
       <c r="D369" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E369">
         <v>3.3</v>
@@ -7056,7 +7053,7 @@
     </row>
     <row r="370" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A370" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B370" t="s">
         <v>77</v>
@@ -7065,7 +7062,7 @@
         <v>10</v>
       </c>
       <c r="D370" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E370">
         <v>15.25</v>
@@ -7073,16 +7070,16 @@
     </row>
     <row r="371" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A371" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B371" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C371">
         <v>210</v>
       </c>
       <c r="D371" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E371">
         <v>2.4500000000000002</v>
@@ -7090,16 +7087,16 @@
     </row>
     <row r="372" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A372" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B372" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C372">
         <v>220</v>
       </c>
       <c r="D372" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E372">
         <v>3.3</v>
@@ -7107,7 +7104,7 @@
     </row>
     <row r="373" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A373" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B373" t="s">
         <v>72</v>
@@ -7116,7 +7113,7 @@
         <v>35</v>
       </c>
       <c r="D373" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E373">
         <v>8.35</v>
@@ -7124,7 +7121,7 @@
     </row>
     <row r="374" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A374" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B374" t="s">
         <v>77</v>
@@ -7133,7 +7130,7 @@
         <v>20</v>
       </c>
       <c r="D374" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E374">
         <v>15.25</v>
@@ -7141,16 +7138,16 @@
     </row>
     <row r="375" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A375" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B375" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C375">
         <v>230</v>
       </c>
       <c r="D375" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E375">
         <v>2.4500000000000002</v>
@@ -7158,16 +7155,16 @@
     </row>
     <row r="376" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A376" t="s">
+        <v>113</v>
+      </c>
+      <c r="B376" t="s">
         <v>114</v>
-      </c>
-      <c r="B376" t="s">
-        <v>115</v>
       </c>
       <c r="C376">
         <v>205</v>
       </c>
       <c r="D376" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E376">
         <v>2.63</v>
@@ -7175,16 +7172,16 @@
     </row>
     <row r="377" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A377" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B377" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C377">
         <v>5</v>
       </c>
       <c r="D377" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E377">
         <v>10.67</v>
@@ -7192,7 +7189,7 @@
     </row>
     <row r="378" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A378" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B378" t="s">
         <v>87</v>
@@ -7201,7 +7198,7 @@
         <v>44</v>
       </c>
       <c r="D378" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E378">
         <v>5</v>
@@ -7209,7 +7206,7 @@
     </row>
     <row r="379" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A379" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B379" t="s">
         <v>77</v>
@@ -7218,7 +7215,7 @@
         <v>10</v>
       </c>
       <c r="D379" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E379">
         <v>15.25</v>
@@ -7226,16 +7223,16 @@
     </row>
     <row r="380" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A380" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B380" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C380">
         <v>230</v>
       </c>
       <c r="D380" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E380">
         <v>2.4500000000000002</v>
@@ -7243,16 +7240,16 @@
     </row>
     <row r="381" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A381" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B381" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C381">
         <v>205</v>
       </c>
       <c r="D381" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E381">
         <v>2.63</v>
@@ -7260,7 +7257,7 @@
     </row>
     <row r="382" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A382" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B382" t="s">
         <v>87</v>
@@ -7269,7 +7266,7 @@
         <v>44</v>
       </c>
       <c r="D382" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E382">
         <v>5</v>
@@ -7277,7 +7274,7 @@
     </row>
     <row r="383" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A383" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B383" t="s">
         <v>88</v>
@@ -7286,7 +7283,7 @@
         <v>62</v>
       </c>
       <c r="D383" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E383">
         <v>5.35</v>
@@ -7294,7 +7291,7 @@
     </row>
     <row r="384" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A384" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B384" t="s">
         <v>77</v>
@@ -7303,7 +7300,7 @@
         <v>10</v>
       </c>
       <c r="D384" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E384">
         <v>15.25</v>
@@ -7311,16 +7308,16 @@
     </row>
     <row r="385" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A385" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B385" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C385">
         <v>210</v>
       </c>
       <c r="D385" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E385">
         <v>2.4500000000000002</v>
@@ -7328,16 +7325,16 @@
     </row>
     <row r="386" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A386" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B386" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C386">
         <v>205</v>
       </c>
       <c r="D386" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E386">
         <v>2.63</v>
@@ -7345,16 +7342,16 @@
     </row>
     <row r="387" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A387" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B387" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C387">
         <v>5</v>
       </c>
       <c r="D387" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E387">
         <v>10.67</v>
@@ -7362,16 +7359,16 @@
     </row>
     <row r="388" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A388" t="s">
+        <v>117</v>
+      </c>
+      <c r="B388" t="s">
         <v>118</v>
-      </c>
-      <c r="B388" t="s">
-        <v>119</v>
       </c>
       <c r="C388">
         <v>5</v>
       </c>
       <c r="D388" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E388">
         <v>2.4</v>
@@ -7379,7 +7376,7 @@
     </row>
     <row r="389" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A389" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B389" t="s">
         <v>77</v>
@@ -7388,7 +7385,7 @@
         <v>10</v>
       </c>
       <c r="D389" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E389">
         <v>15.25</v>
@@ -7396,16 +7393,16 @@
     </row>
     <row r="390" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A390" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B390" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C390">
         <v>230</v>
       </c>
       <c r="D390" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E390">
         <v>2.4500000000000002</v>
@@ -7413,16 +7410,16 @@
     </row>
     <row r="391" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A391" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B391" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C391">
         <v>210</v>
       </c>
       <c r="D391" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E391">
         <v>2.4500000000000002</v>
@@ -7430,7 +7427,7 @@
     </row>
     <row r="392" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A392" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B392" t="s">
         <v>77</v>
@@ -7439,7 +7436,7 @@
         <v>10</v>
       </c>
       <c r="D392" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E392">
         <v>15.25</v>
@@ -7447,16 +7444,16 @@
     </row>
     <row r="393" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A393" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B393" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C393">
         <v>5</v>
       </c>
       <c r="D393" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E393">
         <v>2.4</v>
@@ -7464,16 +7461,16 @@
     </row>
     <row r="394" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A394" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B394" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C394">
         <v>205</v>
       </c>
       <c r="D394" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E394">
         <v>2.63</v>
@@ -7481,7 +7478,7 @@
     </row>
     <row r="395" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A395" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B395" t="s">
         <v>74</v>
@@ -7490,7 +7487,7 @@
         <v>78</v>
       </c>
       <c r="D395" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E395">
         <v>5.5</v>
@@ -7498,16 +7495,16 @@
     </row>
     <row r="396" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A396" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B396" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C396">
         <v>5</v>
       </c>
       <c r="D396" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E396">
         <v>10.67</v>

</xml_diff>